<commit_message>
fixed date typo in metadata
</commit_message>
<xml_diff>
--- a/files/Illumina_Reads_updated_3_20_24.xlsx
+++ b/files/Illumina_Reads_updated_3_20_24.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlanc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruben\bioinfo\SludgeCommunityAnalysis\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{343BA94C-AD46-41C8-9EF9-69CDC8445446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53CC9B2-520C-4895-80E9-23081D0FA2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7559,15 +7559,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7943,10 +7943,10 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P82" sqref="P82"/>
+      <selection pane="bottomRight" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -10936,7 +10936,7 @@
         <v>19</v>
       </c>
       <c r="I77" s="104">
-        <v>45509</v>
+        <v>42221</v>
       </c>
       <c r="J77" s="103" t="s">
         <v>52</v>
@@ -65009,42 +65009,42 @@
     </row>
     <row r="3" spans="1:32" ht="15.75" customHeight="1">
       <c r="A3" s="90"/>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="119" t="s">
         <v>1337</v>
       </c>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
-      <c r="J3" s="118" t="s">
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="121"/>
+      <c r="J3" s="119" t="s">
         <v>1338</v>
       </c>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119"/>
-      <c r="O3" s="119"/>
-      <c r="P3" s="120"/>
-      <c r="R3" s="118" t="s">
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="121"/>
+      <c r="R3" s="119" t="s">
         <v>1339</v>
       </c>
-      <c r="S3" s="119"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="119"/>
-      <c r="V3" s="119"/>
-      <c r="W3" s="119"/>
-      <c r="X3" s="120"/>
-      <c r="Z3" s="118" t="s">
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="121"/>
+      <c r="Z3" s="119" t="s">
         <v>1340</v>
       </c>
-      <c r="AA3" s="119"/>
-      <c r="AB3" s="119"/>
-      <c r="AC3" s="119"/>
-      <c r="AD3" s="119"/>
-      <c r="AE3" s="119"/>
-      <c r="AF3" s="120"/>
+      <c r="AA3" s="120"/>
+      <c r="AB3" s="120"/>
+      <c r="AC3" s="120"/>
+      <c r="AD3" s="120"/>
+      <c r="AE3" s="120"/>
+      <c r="AF3" s="121"/>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1">
       <c r="A4" s="91"/>
@@ -65054,31 +65054,31 @@
       <c r="E4" s="117"/>
       <c r="F4" s="117"/>
       <c r="G4" s="117"/>
-      <c r="H4" s="121"/>
+      <c r="H4" s="122"/>
       <c r="J4" s="117"/>
       <c r="K4" s="117"/>
       <c r="L4" s="117"/>
       <c r="M4" s="117"/>
       <c r="N4" s="117"/>
       <c r="O4" s="117"/>
-      <c r="P4" s="121"/>
+      <c r="P4" s="122"/>
       <c r="R4" s="117"/>
       <c r="S4" s="117"/>
       <c r="T4" s="117"/>
       <c r="U4" s="117"/>
       <c r="V4" s="117"/>
       <c r="W4" s="117"/>
-      <c r="X4" s="121"/>
+      <c r="X4" s="122"/>
       <c r="Z4" s="117"/>
       <c r="AA4" s="117"/>
       <c r="AB4" s="117"/>
       <c r="AC4" s="117"/>
       <c r="AD4" s="117"/>
       <c r="AE4" s="117"/>
-      <c r="AF4" s="121"/>
+      <c r="AF4" s="122"/>
     </row>
     <row r="5" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="118" t="s">
         <v>1341</v>
       </c>
       <c r="B5" s="55"/>
@@ -65856,42 +65856,42 @@
     </row>
     <row r="14" spans="1:32" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:32" ht="14.25" customHeight="1">
-      <c r="B15" s="118" t="s">
+      <c r="B15" s="119" t="s">
         <v>1486</v>
       </c>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="120"/>
-      <c r="J15" s="118" t="s">
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="121"/>
+      <c r="J15" s="119" t="s">
         <v>1487</v>
       </c>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
-      <c r="O15" s="119"/>
-      <c r="P15" s="120"/>
-      <c r="R15" s="118" t="s">
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="121"/>
+      <c r="R15" s="119" t="s">
         <v>1488</v>
       </c>
-      <c r="S15" s="119"/>
-      <c r="T15" s="119"/>
-      <c r="U15" s="119"/>
-      <c r="V15" s="119"/>
-      <c r="W15" s="119"/>
-      <c r="X15" s="120"/>
-      <c r="Z15" s="118" t="s">
+      <c r="S15" s="120"/>
+      <c r="T15" s="120"/>
+      <c r="U15" s="120"/>
+      <c r="V15" s="120"/>
+      <c r="W15" s="120"/>
+      <c r="X15" s="121"/>
+      <c r="Z15" s="119" t="s">
         <v>1489</v>
       </c>
-      <c r="AA15" s="119"/>
-      <c r="AB15" s="119"/>
-      <c r="AC15" s="119"/>
-      <c r="AD15" s="119"/>
-      <c r="AE15" s="119"/>
-      <c r="AF15" s="120"/>
+      <c r="AA15" s="120"/>
+      <c r="AB15" s="120"/>
+      <c r="AC15" s="120"/>
+      <c r="AD15" s="120"/>
+      <c r="AE15" s="120"/>
+      <c r="AF15" s="121"/>
     </row>
     <row r="16" spans="1:32" ht="14.25" customHeight="1">
       <c r="B16" s="117"/>
@@ -65900,28 +65900,28 @@
       <c r="E16" s="117"/>
       <c r="F16" s="117"/>
       <c r="G16" s="117"/>
-      <c r="H16" s="121"/>
+      <c r="H16" s="122"/>
       <c r="J16" s="117"/>
       <c r="K16" s="117"/>
       <c r="L16" s="117"/>
       <c r="M16" s="117"/>
       <c r="N16" s="117"/>
       <c r="O16" s="117"/>
-      <c r="P16" s="121"/>
+      <c r="P16" s="122"/>
       <c r="R16" s="117"/>
       <c r="S16" s="117"/>
       <c r="T16" s="117"/>
       <c r="U16" s="117"/>
       <c r="V16" s="117"/>
       <c r="W16" s="117"/>
-      <c r="X16" s="121"/>
+      <c r="X16" s="122"/>
       <c r="Z16" s="117"/>
       <c r="AA16" s="117"/>
       <c r="AB16" s="117"/>
       <c r="AC16" s="117"/>
       <c r="AD16" s="117"/>
       <c r="AE16" s="117"/>
-      <c r="AF16" s="121"/>
+      <c r="AF16" s="122"/>
     </row>
     <row r="17" spans="2:32" ht="14.25" customHeight="1">
       <c r="B17" s="55"/>
@@ -67674,16 +67674,16 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Z15:AF16"/>
+    <mergeCell ref="B3:H4"/>
+    <mergeCell ref="J3:P4"/>
+    <mergeCell ref="R3:X4"/>
+    <mergeCell ref="Z3:AF4"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="B15:H16"/>
     <mergeCell ref="J15:P16"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="R15:X16"/>
-    <mergeCell ref="Z15:AF16"/>
-    <mergeCell ref="B3:H4"/>
-    <mergeCell ref="J3:P4"/>
-    <mergeCell ref="R3:X4"/>
-    <mergeCell ref="Z3:AF4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>